<commit_message>
27 maret sebelum pulang kantor
</commit_message>
<xml_diff>
--- a/2021 - 2022/1. Laporan Kegiatan Prakom Januari 2021 - Desember 2022_Debi Tomika.xlsx
+++ b/2021 - 2022/1. Laporan Kegiatan Prakom Januari 2021 - Desember 2022_Debi Tomika.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E6173D-4893-48C6-82C3-65DAB7DDE891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1608F89D-08E2-43B0-B6A5-B5E2AC54EAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -731,6 +731,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>) Pengolahan Data</t>
     </r>
@@ -1206,6 +1207,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -1409,11 +1411,26 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1424,26 +1441,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1731,10 +1733,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:V164"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A110" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E117" sqref="E117"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A121" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1750,16 +1755,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1978,25 +1983,25 @@
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="22" t="s">
         <v>272</v>
       </c>
-      <c r="F19" s="20" t="s">
+      <c r="F19" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="20" t="s">
+      <c r="G19" s="22" t="s">
         <v>14</v>
       </c>
       <c r="H19" s="18" t="s">
@@ -2004,13 +2009,13 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
       <c r="H20" s="18" t="s">
         <v>16</v>
       </c>
@@ -2042,27 +2047,27 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="23"/>
-    </row>
-    <row r="23" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="28"/>
+    </row>
+    <row r="23" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>1</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="26"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="25"/>
       <c r="F23" s="13">
         <v>25</v>
       </c>
@@ -2075,16 +2080,16 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="23" t="s">
         <v>252</v>
       </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="26"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="25"/>
     </row>
     <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
@@ -2096,7 +2101,7 @@
       <c r="C25" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="29" t="s">
+      <c r="D25" s="19" t="s">
         <v>229</v>
       </c>
       <c r="E25" s="6" t="s">
@@ -2113,7 +2118,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>2</v>
       </c>
@@ -2141,18 +2146,18 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="23" t="s">
         <v>256</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="26"/>
-    </row>
-    <row r="28" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="25"/>
+    </row>
+    <row r="28" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>1</v>
       </c>
@@ -2179,7 +2184,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>2</v>
       </c>
@@ -2206,7 +2211,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>3</v>
       </c>
@@ -2233,7 +2238,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>4</v>
       </c>
@@ -2260,7 +2265,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>5</v>
       </c>
@@ -2270,7 +2275,7 @@
       <c r="C32" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="29" t="s">
+      <c r="D32" s="19" t="s">
         <v>53</v>
       </c>
       <c r="E32" s="6" t="s">
@@ -2287,7 +2292,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>6</v>
       </c>
@@ -2314,7 +2319,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>7</v>
       </c>
@@ -2324,7 +2329,7 @@
       <c r="C34" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="29" t="s">
+      <c r="D34" s="19" t="s">
         <v>56</v>
       </c>
       <c r="E34" s="6" t="s">
@@ -2341,7 +2346,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>8</v>
       </c>
@@ -2351,7 +2356,7 @@
       <c r="C35" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D35" s="29" t="s">
+      <c r="D35" s="19" t="s">
         <v>57</v>
       </c>
       <c r="E35" s="6" t="s">
@@ -2378,7 +2383,7 @@
       <c r="C36" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D36" s="29" t="s">
+      <c r="D36" s="19" t="s">
         <v>222</v>
       </c>
       <c r="E36" s="6" t="s">
@@ -2395,7 +2400,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>10</v>
       </c>
@@ -2405,7 +2410,7 @@
       <c r="C37" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D37" s="29" t="s">
+      <c r="D37" s="19" t="s">
         <v>223</v>
       </c>
       <c r="E37" s="6" t="s">
@@ -2432,7 +2437,7 @@
       <c r="C38" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D38" s="29" t="s">
+      <c r="D38" s="19" t="s">
         <v>224</v>
       </c>
       <c r="E38" s="6" t="s">
@@ -2476,7 +2481,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>13</v>
       </c>
@@ -2503,19 +2508,19 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="24" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="23" t="s">
         <v>253</v>
       </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="26"/>
-    </row>
-    <row r="42" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="25"/>
+    </row>
+    <row r="42" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>1</v>
       </c>
@@ -2525,7 +2530,7 @@
       <c r="C42" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D42" s="29" t="s">
+      <c r="D42" s="19" t="s">
         <v>227</v>
       </c>
       <c r="E42" s="6" t="s">
@@ -2542,7 +2547,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>2</v>
       </c>
@@ -2552,7 +2557,7 @@
       <c r="C43" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D43" s="29" t="s">
+      <c r="D43" s="19" t="s">
         <v>227</v>
       </c>
       <c r="E43" s="6" t="s">
@@ -2569,7 +2574,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>3</v>
       </c>
@@ -2579,7 +2584,7 @@
       <c r="C44" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D44" s="29" t="s">
+      <c r="D44" s="19" t="s">
         <v>228</v>
       </c>
       <c r="E44" s="6" t="s">
@@ -2596,7 +2601,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>4</v>
       </c>
@@ -2606,7 +2611,7 @@
       <c r="C45" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D45" s="29" t="s">
+      <c r="D45" s="19" t="s">
         <v>228</v>
       </c>
       <c r="E45" s="6" t="s">
@@ -2623,7 +2628,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>5</v>
       </c>
@@ -2633,7 +2638,7 @@
       <c r="C46" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D46" s="29" t="s">
+      <c r="D46" s="19" t="s">
         <v>230</v>
       </c>
       <c r="E46" s="6" t="s">
@@ -2650,7 +2655,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>6</v>
       </c>
@@ -2660,7 +2665,7 @@
       <c r="C47" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D47" s="29" t="s">
+      <c r="D47" s="19" t="s">
         <v>230</v>
       </c>
       <c r="E47" s="6" t="s">
@@ -2677,7 +2682,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>7</v>
       </c>
@@ -2687,7 +2692,7 @@
       <c r="C48" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D48" s="29" t="s">
+      <c r="D48" s="19" t="s">
         <v>231</v>
       </c>
       <c r="E48" s="6" t="s">
@@ -2704,7 +2709,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>8</v>
       </c>
@@ -2714,7 +2719,7 @@
       <c r="C49" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D49" s="29" t="s">
+      <c r="D49" s="19" t="s">
         <v>231</v>
       </c>
       <c r="E49" s="6" t="s">
@@ -2731,7 +2736,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>9</v>
       </c>
@@ -2741,7 +2746,7 @@
       <c r="C50" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="29" t="s">
+      <c r="D50" s="19" t="s">
         <v>232</v>
       </c>
       <c r="E50" s="6" t="s">
@@ -2758,7 +2763,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>10</v>
       </c>
@@ -2768,7 +2773,7 @@
       <c r="C51" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D51" s="29" t="s">
+      <c r="D51" s="19" t="s">
         <v>232</v>
       </c>
       <c r="E51" s="6" t="s">
@@ -2785,7 +2790,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>11</v>
       </c>
@@ -2795,7 +2800,7 @@
       <c r="C52" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D52" s="29" t="s">
+      <c r="D52" s="19" t="s">
         <v>233</v>
       </c>
       <c r="E52" s="6" t="s">
@@ -2822,7 +2827,7 @@
       <c r="C53" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D53" s="29" t="s">
+      <c r="D53" s="19" t="s">
         <v>233</v>
       </c>
       <c r="E53" s="6" t="s">
@@ -2839,7 +2844,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>13</v>
       </c>
@@ -2849,7 +2854,7 @@
       <c r="C54" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D54" s="29" t="s">
+      <c r="D54" s="19" t="s">
         <v>234</v>
       </c>
       <c r="E54" s="6" t="s">
@@ -2866,7 +2871,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>14</v>
       </c>
@@ -2876,7 +2881,7 @@
       <c r="C55" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D55" s="29" t="s">
+      <c r="D55" s="19" t="s">
         <v>234</v>
       </c>
       <c r="E55" s="6" t="s">
@@ -2893,7 +2898,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>15</v>
       </c>
@@ -2903,7 +2908,7 @@
       <c r="C56" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D56" s="29" t="s">
+      <c r="D56" s="19" t="s">
         <v>235</v>
       </c>
       <c r="E56" s="6" t="s">
@@ -2920,7 +2925,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>16</v>
       </c>
@@ -2930,7 +2935,7 @@
       <c r="C57" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D57" s="29" t="s">
+      <c r="D57" s="19" t="s">
         <v>235</v>
       </c>
       <c r="E57" s="6" t="s">
@@ -2947,7 +2952,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>17</v>
       </c>
@@ -2957,7 +2962,7 @@
       <c r="C58" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D58" s="29" t="s">
+      <c r="D58" s="19" t="s">
         <v>236</v>
       </c>
       <c r="E58" s="6" t="s">
@@ -2974,7 +2979,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>18</v>
       </c>
@@ -2984,7 +2989,7 @@
       <c r="C59" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D59" s="29" t="s">
+      <c r="D59" s="19" t="s">
         <v>236</v>
       </c>
       <c r="E59" s="6" t="s">
@@ -3001,7 +3006,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>19</v>
       </c>
@@ -3011,7 +3016,7 @@
       <c r="C60" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D60" s="29" t="s">
+      <c r="D60" s="19" t="s">
         <v>237</v>
       </c>
       <c r="E60" s="6" t="s">
@@ -3028,7 +3033,7 @@
         <v>0.16500000000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>20</v>
       </c>
@@ -3038,7 +3043,7 @@
       <c r="C61" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D61" s="29" t="s">
+      <c r="D61" s="19" t="s">
         <v>237</v>
       </c>
       <c r="E61" s="6" t="s">
@@ -3055,7 +3060,7 @@
         <v>0.16500000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>21</v>
       </c>
@@ -3065,7 +3070,7 @@
       <c r="C62" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D62" s="29" t="s">
+      <c r="D62" s="19" t="s">
         <v>93</v>
       </c>
       <c r="E62" s="6" t="s">
@@ -3082,7 +3087,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>22</v>
       </c>
@@ -3092,7 +3097,7 @@
       <c r="C63" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D63" s="29" t="s">
+      <c r="D63" s="19" t="s">
         <v>94</v>
       </c>
       <c r="E63" s="6" t="s">
@@ -3109,7 +3114,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>23</v>
       </c>
@@ -3119,7 +3124,7 @@
       <c r="C64" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D64" s="29" t="s">
+      <c r="D64" s="19" t="s">
         <v>97</v>
       </c>
       <c r="E64" s="6" t="s">
@@ -3136,7 +3141,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>24</v>
       </c>
@@ -3146,7 +3151,7 @@
       <c r="C65" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D65" s="29" t="s">
+      <c r="D65" s="19" t="s">
         <v>98</v>
       </c>
       <c r="E65" s="6" t="s">
@@ -3163,7 +3168,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>25</v>
       </c>
@@ -3173,7 +3178,7 @@
       <c r="C66" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D66" s="29" t="s">
+      <c r="D66" s="19" t="s">
         <v>101</v>
       </c>
       <c r="E66" s="6" t="s">
@@ -3190,7 +3195,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>26</v>
       </c>
@@ -3200,7 +3205,7 @@
       <c r="C67" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D67" s="29" t="s">
+      <c r="D67" s="19" t="s">
         <v>54</v>
       </c>
       <c r="E67" s="6" t="s">
@@ -3217,7 +3222,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>27</v>
       </c>
@@ -3227,7 +3232,7 @@
       <c r="C68" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D68" s="29" t="s">
+      <c r="D68" s="19" t="s">
         <v>54</v>
       </c>
       <c r="E68" s="6" t="s">
@@ -3244,7 +3249,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>28</v>
       </c>
@@ -3254,7 +3259,7 @@
       <c r="C69" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D69" s="29" t="s">
+      <c r="D69" s="19" t="s">
         <v>104</v>
       </c>
       <c r="E69" s="6" t="s">
@@ -3271,7 +3276,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>29</v>
       </c>
@@ -3281,7 +3286,7 @@
       <c r="C70" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D70" s="29" t="s">
+      <c r="D70" s="19" t="s">
         <v>108</v>
       </c>
       <c r="E70" s="6" t="s">
@@ -3298,7 +3303,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>30</v>
       </c>
@@ -3308,7 +3313,7 @@
       <c r="C71" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D71" s="30" t="s">
+      <c r="D71" s="20" t="s">
         <v>109</v>
       </c>
       <c r="E71" s="6" t="s">
@@ -3325,7 +3330,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>31</v>
       </c>
@@ -3335,7 +3340,7 @@
       <c r="C72" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D72" s="29" t="s">
+      <c r="D72" s="19" t="s">
         <v>111</v>
       </c>
       <c r="E72" s="6" t="s">
@@ -3352,7 +3357,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>32</v>
       </c>
@@ -3362,7 +3367,7 @@
       <c r="C73" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D73" s="30" t="s">
+      <c r="D73" s="20" t="s">
         <v>113</v>
       </c>
       <c r="E73" s="6" t="s">
@@ -3379,7 +3384,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>33</v>
       </c>
@@ -3389,7 +3394,7 @@
       <c r="C74" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D74" s="29" t="s">
+      <c r="D74" s="19" t="s">
         <v>56</v>
       </c>
       <c r="E74" s="6" t="s">
@@ -3406,7 +3411,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>34</v>
       </c>
@@ -3416,7 +3421,7 @@
       <c r="C75" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D75" s="29" t="s">
+      <c r="D75" s="19" t="s">
         <v>116</v>
       </c>
       <c r="E75" s="6" t="s">
@@ -3433,7 +3438,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>35</v>
       </c>
@@ -3443,7 +3448,7 @@
       <c r="C76" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D76" s="30" t="s">
+      <c r="D76" s="20" t="s">
         <v>118</v>
       </c>
       <c r="E76" s="6" t="s">
@@ -3460,7 +3465,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>36</v>
       </c>
@@ -3470,7 +3475,7 @@
       <c r="C77" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D77" s="29" t="s">
+      <c r="D77" s="19" t="s">
         <v>57</v>
       </c>
       <c r="E77" s="6" t="s">
@@ -3487,7 +3492,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>37</v>
       </c>
@@ -3497,7 +3502,7 @@
       <c r="C78" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D78" s="30" t="s">
+      <c r="D78" s="20" t="s">
         <v>57</v>
       </c>
       <c r="E78" s="6" t="s">
@@ -3514,7 +3519,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>38</v>
       </c>
@@ -3524,7 +3529,7 @@
       <c r="C79" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D79" s="29" t="s">
+      <c r="D79" s="19" t="s">
         <v>122</v>
       </c>
       <c r="E79" s="6" t="s">
@@ -3541,7 +3546,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>39</v>
       </c>
@@ -3551,7 +3556,7 @@
       <c r="C80" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D80" s="29" t="s">
+      <c r="D80" s="19" t="s">
         <v>124</v>
       </c>
       <c r="E80" s="6" t="s">
@@ -3568,7 +3573,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>40</v>
       </c>
@@ -3578,7 +3583,7 @@
       <c r="C81" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D81" s="29" t="s">
+      <c r="D81" s="19" t="s">
         <v>124</v>
       </c>
       <c r="E81" s="6" t="s">
@@ -3595,7 +3600,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>41</v>
       </c>
@@ -3605,7 +3610,7 @@
       <c r="C82" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D82" s="29" t="s">
+      <c r="D82" s="19" t="s">
         <v>127</v>
       </c>
       <c r="E82" s="6" t="s">
@@ -3622,7 +3627,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>42</v>
       </c>
@@ -3632,7 +3637,7 @@
       <c r="C83" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D83" s="29" t="s">
+      <c r="D83" s="19" t="s">
         <v>239</v>
       </c>
       <c r="E83" s="6" t="s">
@@ -3649,7 +3654,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>43</v>
       </c>
@@ -3659,7 +3664,7 @@
       <c r="C84" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D84" s="29" t="s">
+      <c r="D84" s="19" t="s">
         <v>240</v>
       </c>
       <c r="E84" s="6" t="s">
@@ -3676,7 +3681,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>44</v>
       </c>
@@ -3686,7 +3691,7 @@
       <c r="C85" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D85" s="29" t="s">
+      <c r="D85" s="19" t="s">
         <v>241</v>
       </c>
       <c r="E85" s="6" t="s">
@@ -3703,7 +3708,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>45</v>
       </c>
@@ -3713,7 +3718,7 @@
       <c r="C86" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D86" s="29" t="s">
+      <c r="D86" s="19" t="s">
         <v>242</v>
       </c>
       <c r="E86" s="6" t="s">
@@ -3730,7 +3735,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>46</v>
       </c>
@@ -3740,7 +3745,7 @@
       <c r="C87" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D87" s="29" t="s">
+      <c r="D87" s="19" t="s">
         <v>243</v>
       </c>
       <c r="E87" s="6" t="s">
@@ -3767,7 +3772,7 @@
       <c r="C88" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D88" s="29" t="s">
+      <c r="D88" s="19" t="s">
         <v>244</v>
       </c>
       <c r="E88" s="6" t="s">
@@ -3784,7 +3789,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>48</v>
       </c>
@@ -3794,7 +3799,7 @@
       <c r="C89" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D89" s="29" t="s">
+      <c r="D89" s="19" t="s">
         <v>245</v>
       </c>
       <c r="E89" s="6" t="s">
@@ -3811,7 +3816,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>49</v>
       </c>
@@ -3821,7 +3826,7 @@
       <c r="C90" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D90" s="29" t="s">
+      <c r="D90" s="19" t="s">
         <v>247</v>
       </c>
       <c r="E90" s="6" t="s">
@@ -3838,7 +3843,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>50</v>
       </c>
@@ -3848,7 +3853,7 @@
       <c r="C91" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D91" s="29" t="s">
+      <c r="D91" s="19" t="s">
         <v>246</v>
       </c>
       <c r="E91" s="6" t="s">
@@ -3865,7 +3870,7 @@
         <v>0.16500000000000001</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>51</v>
       </c>
@@ -3875,7 +3880,7 @@
       <c r="C92" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D92" s="29" t="s">
+      <c r="D92" s="19" t="s">
         <v>198</v>
       </c>
       <c r="E92" s="6" t="s">
@@ -3892,7 +3897,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>52</v>
       </c>
@@ -3902,7 +3907,7 @@
       <c r="C93" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D93" s="29" t="s">
+      <c r="D93" s="19" t="s">
         <v>199</v>
       </c>
       <c r="E93" s="6" t="s">
@@ -3919,7 +3924,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>53</v>
       </c>
@@ -3929,7 +3934,7 @@
       <c r="C94" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D94" s="29" t="s">
+      <c r="D94" s="19" t="s">
         <v>200</v>
       </c>
       <c r="E94" s="6" t="s">
@@ -3946,7 +3951,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>54</v>
       </c>
@@ -3956,7 +3961,7 @@
       <c r="C95" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D95" s="29" t="s">
+      <c r="D95" s="19" t="s">
         <v>201</v>
       </c>
       <c r="E95" s="6" t="s">
@@ -3973,7 +3978,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>55</v>
       </c>
@@ -3983,7 +3988,7 @@
       <c r="C96" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D96" s="29" t="s">
+      <c r="D96" s="19" t="s">
         <v>202</v>
       </c>
       <c r="E96" s="6" t="s">
@@ -4000,7 +4005,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="97" spans="1:22" ht="57" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:22" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>56</v>
       </c>
@@ -4010,7 +4015,7 @@
       <c r="C97" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D97" s="29" t="s">
+      <c r="D97" s="19" t="s">
         <v>202</v>
       </c>
       <c r="E97" s="6" t="s">
@@ -4027,7 +4032,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="98" spans="1:22" ht="57" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:22" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>57</v>
       </c>
@@ -4037,7 +4042,7 @@
       <c r="C98" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D98" s="29" t="s">
+      <c r="D98" s="19" t="s">
         <v>203</v>
       </c>
       <c r="E98" s="6" t="s">
@@ -4054,7 +4059,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="99" spans="1:22" ht="57" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:22" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>58</v>
       </c>
@@ -4064,7 +4069,7 @@
       <c r="C99" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D99" s="29" t="s">
+      <c r="D99" s="19" t="s">
         <v>206</v>
       </c>
       <c r="E99" s="6" t="s">
@@ -4081,7 +4086,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="100" spans="1:22" ht="57" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:22" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>59</v>
       </c>
@@ -4091,7 +4096,7 @@
       <c r="C100" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D100" s="29" t="s">
+      <c r="D100" s="19" t="s">
         <v>205</v>
       </c>
       <c r="E100" s="6" t="s">
@@ -4108,7 +4113,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="101" spans="1:22" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:22" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>60</v>
       </c>
@@ -4118,7 +4123,7 @@
       <c r="C101" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D101" s="29" t="s">
+      <c r="D101" s="19" t="s">
         <v>207</v>
       </c>
       <c r="E101" s="6" t="s">
@@ -4135,7 +4140,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="102" spans="1:22" ht="57" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:22" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>61</v>
       </c>
@@ -4145,7 +4150,7 @@
       <c r="C102" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D102" s="29" t="s">
+      <c r="D102" s="19" t="s">
         <v>207</v>
       </c>
       <c r="E102" s="6" t="s">
@@ -4162,7 +4167,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="103" spans="1:22" ht="57" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:22" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <v>62</v>
       </c>
@@ -4172,7 +4177,7 @@
       <c r="C103" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D103" s="29" t="s">
+      <c r="D103" s="19" t="s">
         <v>208</v>
       </c>
       <c r="E103" s="6" t="s">
@@ -4189,7 +4194,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="104" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A104" s="31" t="s">
         <v>254</v>
       </c>
@@ -4215,7 +4220,7 @@
       <c r="U104" s="8"/>
       <c r="V104" s="8"/>
     </row>
-    <row r="105" spans="1:22" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:22" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A105" s="9">
         <v>1</v>
       </c>
@@ -4256,7 +4261,7 @@
       <c r="U105" s="8"/>
       <c r="V105" s="8"/>
     </row>
-    <row r="106" spans="1:22" ht="57" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:22" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A106" s="9">
         <v>2</v>
       </c>
@@ -4297,7 +4302,7 @@
       <c r="U106" s="8"/>
       <c r="V106" s="8"/>
     </row>
-    <row r="107" spans="1:22" ht="57" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:22" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A107" s="9">
         <v>3</v>
       </c>
@@ -4379,19 +4384,19 @@
       <c r="U108" s="8"/>
       <c r="V108" s="8"/>
     </row>
-    <row r="109" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="24" t="s">
+    <row r="109" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A109" s="23" t="s">
         <v>255</v>
       </c>
-      <c r="B109" s="25"/>
-      <c r="C109" s="25"/>
-      <c r="D109" s="25"/>
-      <c r="E109" s="25"/>
-      <c r="F109" s="25"/>
-      <c r="G109" s="25"/>
-      <c r="H109" s="26"/>
-    </row>
-    <row r="110" spans="1:22" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B109" s="24"/>
+      <c r="C109" s="24"/>
+      <c r="D109" s="24"/>
+      <c r="E109" s="24"/>
+      <c r="F109" s="24"/>
+      <c r="G109" s="24"/>
+      <c r="H109" s="25"/>
+    </row>
+    <row r="110" spans="1:22" ht="57" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>1</v>
       </c>
@@ -4401,7 +4406,7 @@
       <c r="C110" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="D110" s="29" t="s">
+      <c r="D110" s="19" t="s">
         <v>211</v>
       </c>
       <c r="E110" s="6" t="s">
@@ -4418,7 +4423,7 @@
         <v>0.16500000000000001</v>
       </c>
     </row>
-    <row r="111" spans="1:22" ht="57" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:22" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <v>2</v>
       </c>
@@ -4428,7 +4433,7 @@
       <c r="C111" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="D111" s="29" t="s">
+      <c r="D111" s="19" t="s">
         <v>213</v>
       </c>
       <c r="E111" s="6" t="s">
@@ -4446,18 +4451,18 @@
       </c>
     </row>
     <row r="112" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A112" s="24" t="s">
+      <c r="A112" s="23" t="s">
         <v>257</v>
       </c>
-      <c r="B112" s="25"/>
-      <c r="C112" s="25"/>
-      <c r="D112" s="25"/>
-      <c r="E112" s="25"/>
-      <c r="F112" s="25"/>
-      <c r="G112" s="25"/>
-      <c r="H112" s="26"/>
-    </row>
-    <row r="113" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+      <c r="B112" s="24"/>
+      <c r="C112" s="24"/>
+      <c r="D112" s="24"/>
+      <c r="E112" s="24"/>
+      <c r="F112" s="24"/>
+      <c r="G112" s="24"/>
+      <c r="H112" s="25"/>
+    </row>
+    <row r="113" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>1</v>
       </c>
@@ -4467,7 +4472,7 @@
       <c r="C113" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D113" s="29" t="s">
+      <c r="D113" s="19" t="s">
         <v>164</v>
       </c>
       <c r="E113" s="6" t="s">
@@ -4484,7 +4489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <v>2</v>
       </c>
@@ -4494,7 +4499,7 @@
       <c r="C114" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D114" s="29" t="s">
+      <c r="D114" s="19" t="s">
         <v>158</v>
       </c>
       <c r="E114" s="6" t="s">
@@ -4511,7 +4516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
         <v>3</v>
       </c>
@@ -4521,7 +4526,7 @@
       <c r="C115" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D115" s="29" t="s">
+      <c r="D115" s="19" t="s">
         <v>162</v>
       </c>
       <c r="E115" s="6" t="s">
@@ -4538,7 +4543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>4</v>
       </c>
@@ -4548,7 +4553,7 @@
       <c r="C116" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D116" s="29" t="s">
+      <c r="D116" s="19" t="s">
         <v>104</v>
       </c>
       <c r="E116" s="6" t="s">
@@ -4575,7 +4580,7 @@
       <c r="C117" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D117" s="29" t="s">
+      <c r="D117" s="19" t="s">
         <v>169</v>
       </c>
       <c r="E117" s="6" t="s">
@@ -4592,7 +4597,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <v>6</v>
       </c>
@@ -4602,7 +4607,7 @@
       <c r="C118" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="D118" s="29" t="s">
+      <c r="D118" s="19" t="s">
         <v>170</v>
       </c>
       <c r="E118" s="6" t="s">
@@ -4619,7 +4624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
         <v>7</v>
       </c>
@@ -4629,7 +4634,7 @@
       <c r="C119" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D119" s="29" t="s">
+      <c r="D119" s="19" t="s">
         <v>172</v>
       </c>
       <c r="E119" s="6" t="s">
@@ -4646,7 +4651,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
         <v>8</v>
       </c>
@@ -4656,7 +4661,7 @@
       <c r="C120" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D120" s="29" t="s">
+      <c r="D120" s="19" t="s">
         <v>178</v>
       </c>
       <c r="E120" s="6" t="s">
@@ -4673,7 +4678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
         <v>9</v>
       </c>
@@ -4683,7 +4688,7 @@
       <c r="C121" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D121" s="29" t="s">
+      <c r="D121" s="19" t="s">
         <v>174</v>
       </c>
       <c r="E121" s="6" t="s">
@@ -4700,7 +4705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
         <v>10</v>
       </c>
@@ -4710,7 +4715,7 @@
       <c r="C122" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D122" s="29" t="s">
+      <c r="D122" s="19" t="s">
         <v>176</v>
       </c>
       <c r="E122" s="6" t="s">
@@ -4727,7 +4732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
         <v>11</v>
       </c>
@@ -4737,7 +4742,7 @@
       <c r="C123" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D123" s="29" t="s">
+      <c r="D123" s="19" t="s">
         <v>181</v>
       </c>
       <c r="E123" s="6" t="s">
@@ -4754,7 +4759,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A124" s="4">
         <v>12</v>
       </c>
@@ -4764,7 +4769,7 @@
       <c r="C124" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="D124" s="29" t="s">
+      <c r="D124" s="19" t="s">
         <v>216</v>
       </c>
       <c r="E124" s="6" t="s">
@@ -4781,7 +4786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A125" s="4">
         <v>13</v>
       </c>
@@ -4791,7 +4796,7 @@
       <c r="C125" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D125" s="29" t="s">
+      <c r="D125" s="19" t="s">
         <v>182</v>
       </c>
       <c r="E125" s="6" t="s">
@@ -4808,7 +4813,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A126" s="4">
         <v>14</v>
       </c>
@@ -4818,7 +4823,7 @@
       <c r="C126" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D126" s="29" t="s">
+      <c r="D126" s="19" t="s">
         <v>184</v>
       </c>
       <c r="E126" s="6" t="s">
@@ -4836,15 +4841,15 @@
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A127" s="28" t="s">
+      <c r="A127" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B127" s="28"/>
-      <c r="C127" s="28"/>
-      <c r="D127" s="28"/>
-      <c r="E127" s="28"/>
-      <c r="F127" s="28"/>
-      <c r="G127" s="28"/>
+      <c r="B127" s="30"/>
+      <c r="C127" s="30"/>
+      <c r="D127" s="30"/>
+      <c r="E127" s="30"/>
+      <c r="F127" s="30"/>
+      <c r="G127" s="30"/>
       <c r="H127" s="15">
         <f>SUM(H23:H126)</f>
         <v>76.744999999999962</v>
@@ -4878,11 +4883,11 @@
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
-      <c r="F130" s="19" t="s">
+      <c r="F130" s="21" t="s">
         <v>258</v>
       </c>
-      <c r="G130" s="19"/>
-      <c r="H130" s="19"/>
+      <c r="G130" s="21"/>
+      <c r="H130" s="21"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
@@ -4890,11 +4895,11 @@
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
-      <c r="F131" s="19" t="s">
+      <c r="F131" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="G131" s="19"/>
-      <c r="H131" s="19"/>
+      <c r="G131" s="21"/>
+      <c r="H131" s="21"/>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
@@ -4942,11 +4947,11 @@
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
       <c r="E136" s="1"/>
-      <c r="F136" s="19" t="s">
+      <c r="F136" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="G136" s="19"/>
-      <c r="H136" s="19"/>
+      <c r="G136" s="21"/>
+      <c r="H136" s="21"/>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
@@ -4954,11 +4959,11 @@
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
-      <c r="F137" s="19" t="s">
+      <c r="F137" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="G137" s="19"/>
-      <c r="H137" s="19"/>
+      <c r="G137" s="21"/>
+      <c r="H137" s="21"/>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
@@ -5256,9 +5261,6 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="108" max="16383" man="1"/>
-  </rowBreaks>
+  <pageSetup paperSize="9" scale="96" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>